<commit_message>
modified test.py for parsing 3 keywords
</commit_message>
<xml_diff>
--- a/crypto.xlsx
+++ b/crypto.xlsx
@@ -14,17 +14,53 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="150">
   <si>
     <t>Quantum cryptography</t>
   </si>
   <si>
-    <t>quantum cryptography</t>
+    <t>IoT security</t>
+  </si>
+  <si>
+    <t>Automated and adaptive networks</t>
   </si>
   <si>
     <t>quantum key distribution</t>
   </si>
   <si>
+    <t>cryptography</t>
+  </si>
+  <si>
+    <t>post-quantum cryptography</t>
+  </si>
+  <si>
+    <t>lattice-based cryptography</t>
+  </si>
+  <si>
+    <t>cryptanalysis</t>
+  </si>
+  <si>
+    <t>quantum information</t>
+  </si>
+  <si>
+    <t>applied computer science</t>
+  </si>
+  <si>
+    <t>privacy-preserving protocols</t>
+  </si>
+  <si>
+    <t>blockchain</t>
+  </si>
+  <si>
+    <t>learning with errors</t>
+  </si>
+  <si>
+    <t>isogenies</t>
+  </si>
+  <si>
+    <t>quirk</t>
+  </si>
+  <si>
     <t>security</t>
   </si>
   <si>
@@ -76,33 +112,21 @@
     <t>ntru</t>
   </si>
   <si>
-    <t>cryptography</t>
-  </si>
-  <si>
     <t>lattice cryptography</t>
   </si>
   <si>
-    <t>post-quantum cryptography</t>
-  </si>
-  <si>
     <t>digital signatures</t>
   </si>
   <si>
     <t>public key encryption</t>
   </si>
   <si>
-    <t>cryptanalysis</t>
-  </si>
-  <si>
     <t>key establishment</t>
   </si>
   <si>
     <t>elliptic curve cryptography</t>
   </si>
   <si>
-    <t>applied computer science</t>
-  </si>
-  <si>
     <t>applied mathematics not elsewhere classified</t>
   </si>
   <si>
@@ -112,9 +136,6 @@
     <t>cybersecurity</t>
   </si>
   <si>
-    <t>lattice-based cryptography</t>
-  </si>
-  <si>
     <t>zero-knowledge proofs</t>
   </si>
   <si>
@@ -124,12 +145,6 @@
     <t>group signature</t>
   </si>
   <si>
-    <t>privacy-preserving protocols</t>
-  </si>
-  <si>
-    <t>blockchain</t>
-  </si>
-  <si>
     <t>kvantová kryptografie</t>
   </si>
   <si>
@@ -149,6 +164,306 @@
   </si>
   <si>
     <t>protokol sarg04</t>
+  </si>
+  <si>
+    <t>protocol bb84</t>
+  </si>
+  <si>
+    <t>protocol b92</t>
+  </si>
+  <si>
+    <t>six-state protocol</t>
+  </si>
+  <si>
+    <t>iot</t>
+  </si>
+  <si>
+    <t>internet of things</t>
+  </si>
+  <si>
+    <t>privacy</t>
+  </si>
+  <si>
+    <t>mqtt</t>
+  </si>
+  <si>
+    <t>mosquitto</t>
+  </si>
+  <si>
+    <t>aes</t>
+  </si>
+  <si>
+    <t>eciespy</t>
+  </si>
+  <si>
+    <t>tlsssl</t>
+  </si>
+  <si>
+    <t>rabin</t>
+  </si>
+  <si>
+    <t>raspberry pi</t>
+  </si>
+  <si>
+    <t>internet of things (iot)</t>
+  </si>
+  <si>
+    <t>engineering and technology</t>
+  </si>
+  <si>
+    <t>teknik och teknologier</t>
+  </si>
+  <si>
+    <t>electrical engineering, electronic engineering, information engineering</t>
+  </si>
+  <si>
+    <t>elektroteknik och elektronik</t>
+  </si>
+  <si>
+    <t>uncategorized content</t>
+  </si>
+  <si>
+    <t>threats</t>
+  </si>
+  <si>
+    <t>bluetooth low energy</t>
+  </si>
+  <si>
+    <t>fields of research</t>
+  </si>
+  <si>
+    <t>computer engineering</t>
+  </si>
+  <si>
+    <t>network security</t>
+  </si>
+  <si>
+    <t>information security</t>
+  </si>
+  <si>
+    <t>computer sciences</t>
+  </si>
+  <si>
+    <t>datavetenskap (datalogi)</t>
+  </si>
+  <si>
+    <t>bezpečnost iot</t>
+  </si>
+  <si>
+    <t>edge computing</t>
+  </si>
+  <si>
+    <t>secure outsourcing computation</t>
+  </si>
+  <si>
+    <t>social iot systems</t>
+  </si>
+  <si>
+    <t>blockchains (databases)</t>
+  </si>
+  <si>
+    <t>internet of things  –  security measures</t>
+  </si>
+  <si>
+    <t>data encryption (computer science)</t>
+  </si>
+  <si>
+    <t>openness</t>
+  </si>
+  <si>
+    <t>trust</t>
+  </si>
+  <si>
+    <t>vulnerabilities</t>
+  </si>
+  <si>
+    <t>software</t>
+  </si>
+  <si>
+    <t>architecture</t>
+  </si>
+  <si>
+    <t>constraints</t>
+  </si>
+  <si>
+    <t>design</t>
+  </si>
+  <si>
+    <t>electrical and computer engineering</t>
+  </si>
+  <si>
+    <t>object security</t>
+  </si>
+  <si>
+    <t>cose</t>
+  </si>
+  <si>
+    <t>end-to-end security</t>
+  </si>
+  <si>
+    <t>coap</t>
+  </si>
+  <si>
+    <t>lwm2m</t>
+  </si>
+  <si>
+    <t>ble security</t>
+  </si>
+  <si>
+    <t>big data</t>
+  </si>
+  <si>
+    <t>contextualisation</t>
+  </si>
+  <si>
+    <t>context</t>
+  </si>
+  <si>
+    <t>collision avoidance</t>
+  </si>
+  <si>
+    <t>mechanical engineering</t>
+  </si>
+  <si>
+    <t>metatrader</t>
+  </si>
+  <si>
+    <t>adaptive computing systems</t>
+  </si>
+  <si>
+    <t>computer architecture</t>
+  </si>
+  <si>
+    <t>field programmable gate arrays</t>
+  </si>
+  <si>
+    <t>robotics</t>
+  </si>
+  <si>
+    <t>electrical engineering</t>
+  </si>
+  <si>
+    <t>adaptive boosting adaboost</t>
+  </si>
+  <si>
+    <t>automatic detection</t>
+  </si>
+  <si>
+    <t>classification</t>
+  </si>
+  <si>
+    <t>pattern recognition</t>
+  </si>
+  <si>
+    <t>satellite images</t>
+  </si>
+  <si>
+    <t>land use – remote sensing</t>
+  </si>
+  <si>
+    <t>computer vision</t>
+  </si>
+  <si>
+    <t>wireless communications</t>
+  </si>
+  <si>
+    <t>optical communications</t>
+  </si>
+  <si>
+    <t>beamsteering</t>
+  </si>
+  <si>
+    <t>localization and tracking systems</t>
+  </si>
+  <si>
+    <t>spatial light modulators</t>
+  </si>
+  <si>
+    <t>optical wireless communications</t>
+  </si>
+  <si>
+    <t>adaptive optics</t>
+  </si>
+  <si>
+    <t>ultrafast wireless communications</t>
+  </si>
+  <si>
+    <t>indoor wireless coverage</t>
+  </si>
+  <si>
+    <t>ics security</t>
+  </si>
+  <si>
+    <t>security training</t>
+  </si>
+  <si>
+    <t>security patterns</t>
+  </si>
+  <si>
+    <t>ics security by design</t>
+  </si>
+  <si>
+    <t>personalized training</t>
+  </si>
+  <si>
+    <t>on the job training</t>
+  </si>
+  <si>
+    <t>autonomous vehicles</t>
+  </si>
+  <si>
+    <t>model predictive control  (mpc)</t>
+  </si>
+  <si>
+    <t>sliding mode controller</t>
+  </si>
+  <si>
+    <t>automated vehicles</t>
+  </si>
+  <si>
+    <t>sistema tutor inteligente</t>
+  </si>
+  <si>
+    <t>sti</t>
+  </si>
+  <si>
+    <t>redes som</t>
+  </si>
+  <si>
+    <t>mapas de kohonen</t>
+  </si>
+  <si>
+    <t>sti baseado em redes neurais</t>
+  </si>
+  <si>
+    <t>sti híbrido</t>
+  </si>
+  <si>
+    <t>inteligência artificial</t>
+  </si>
+  <si>
+    <t>ensino a distância</t>
+  </si>
+  <si>
+    <t>intelligent tutoring systems</t>
+  </si>
+  <si>
+    <t>its</t>
+  </si>
+  <si>
+    <t>self organizing maps</t>
+  </si>
+  <si>
+    <t>som</t>
+  </si>
+  <si>
+    <t>kohonen maps</t>
+  </si>
+  <si>
+    <t>its based on neural networks</t>
+  </si>
+  <si>
+    <t>hybrid its</t>
   </si>
 </sst>
 </file>
@@ -506,415 +821,721 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:B51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:4">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:2">
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>55</v>
+      </c>
+      <c r="D5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>7</v>
+      </c>
+      <c r="C6" t="s">
+        <v>56</v>
+      </c>
+      <c r="D6" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>8</v>
+      </c>
+      <c r="C7" t="s">
+        <v>57</v>
+      </c>
+      <c r="D7" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>9</v>
+      </c>
+      <c r="C8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>59</v>
+      </c>
+      <c r="D9" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>60</v>
+      </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2">
+        <v>12</v>
+      </c>
+      <c r="C11" t="s">
+        <v>61</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="1">
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>62</v>
+      </c>
+      <c r="D12" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="1">
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>63</v>
+      </c>
+      <c r="D13" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="1">
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="15" spans="1:2">
+        <v>15</v>
+      </c>
+      <c r="C14" t="s">
+        <v>64</v>
+      </c>
+      <c r="D14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
       <c r="A15" s="1">
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="16" spans="1:2">
+        <v>16</v>
+      </c>
+      <c r="C15" t="s">
+        <v>65</v>
+      </c>
+      <c r="D15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
       <c r="A16" s="1">
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="17" spans="1:2">
+        <v>17</v>
+      </c>
+      <c r="C16" t="s">
+        <v>66</v>
+      </c>
+      <c r="D16" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
       <c r="A17" s="1">
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="18" spans="1:2">
+        <v>18</v>
+      </c>
+      <c r="C17" t="s">
+        <v>67</v>
+      </c>
+      <c r="D17" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
       <c r="A18" s="1">
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:2">
+        <v>19</v>
+      </c>
+      <c r="C18" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
       <c r="A19" s="1">
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="20" spans="1:2">
+        <v>20</v>
+      </c>
+      <c r="C19" t="s">
+        <v>69</v>
+      </c>
+      <c r="D19" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
       <c r="A20" s="1">
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="21" spans="1:2">
+        <v>21</v>
+      </c>
+      <c r="C20" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
       <c r="A21" s="1">
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="22" spans="1:2">
+        <v>22</v>
+      </c>
+      <c r="C21" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:2">
+        <v>23</v>
+      </c>
+      <c r="C22" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:2">
+        <v>24</v>
+      </c>
+      <c r="C23" t="s">
+        <v>73</v>
+      </c>
+      <c r="D23" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="25" spans="1:2">
+        <v>25</v>
+      </c>
+      <c r="C24" t="s">
+        <v>39</v>
+      </c>
+      <c r="D24" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:2">
+        <v>26</v>
+      </c>
+      <c r="C25" t="s">
+        <v>74</v>
+      </c>
+      <c r="D25" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="27" spans="1:2">
+        <v>27</v>
+      </c>
+      <c r="C26" t="s">
+        <v>75</v>
+      </c>
+      <c r="D26" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:2">
+        <v>28</v>
+      </c>
+      <c r="C27" t="s">
+        <v>76</v>
+      </c>
+      <c r="D27" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
       <c r="A28" s="1">
         <v>26</v>
       </c>
       <c r="B28" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="29" spans="1:2">
+        <v>29</v>
+      </c>
+      <c r="C28" t="s">
+        <v>77</v>
+      </c>
+      <c r="D28" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
       <c r="A29" s="1">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="30" spans="1:2">
+        <v>30</v>
+      </c>
+      <c r="C29" t="s">
+        <v>78</v>
+      </c>
+      <c r="D29" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
       <c r="A30" s="1">
         <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="31" spans="1:2">
+        <v>31</v>
+      </c>
+      <c r="C30" t="s">
+        <v>79</v>
+      </c>
+      <c r="D30" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
       <c r="A31" s="1">
         <v>29</v>
       </c>
       <c r="B31" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="32" spans="1:2">
+        <v>32</v>
+      </c>
+      <c r="C31" t="s">
+        <v>80</v>
+      </c>
+      <c r="D31" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="33" spans="1:2">
+        <v>33</v>
+      </c>
+      <c r="C32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D32" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="34" spans="1:2">
+        <v>34</v>
+      </c>
+      <c r="C33" t="s">
+        <v>82</v>
+      </c>
+      <c r="D33" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="35" spans="1:2">
+        <v>35</v>
+      </c>
+      <c r="C34" t="s">
+        <v>83</v>
+      </c>
+      <c r="D34" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="36" spans="1:2">
+        <v>36</v>
+      </c>
+      <c r="C35" t="s">
+        <v>84</v>
+      </c>
+      <c r="D35" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2">
+        <v>37</v>
+      </c>
+      <c r="C36" t="s">
+        <v>85</v>
+      </c>
+      <c r="D36" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="38" spans="1:2">
+        <v>38</v>
+      </c>
+      <c r="C37" t="s">
+        <v>86</v>
+      </c>
+      <c r="D37" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
       <c r="A38" s="1">
         <v>36</v>
       </c>
       <c r="B38" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="39" spans="1:2">
+        <v>39</v>
+      </c>
+      <c r="C38" t="s">
+        <v>87</v>
+      </c>
+      <c r="D38" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
       <c r="A39" s="1">
         <v>37</v>
       </c>
       <c r="B39" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="40" spans="1:2">
+        <v>40</v>
+      </c>
+      <c r="C39" t="s">
+        <v>88</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="41" spans="1:2">
+        <v>41</v>
+      </c>
+      <c r="C40" t="s">
+        <v>89</v>
+      </c>
+      <c r="D40" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="42" spans="1:2">
+        <v>42</v>
+      </c>
+      <c r="C41" t="s">
+        <v>90</v>
+      </c>
+      <c r="D41" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
       <c r="A42" s="1">
         <v>40</v>
       </c>
       <c r="B42" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="43" spans="1:2">
+        <v>43</v>
+      </c>
+      <c r="C42" t="s">
+        <v>91</v>
+      </c>
+      <c r="D42" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="43" spans="1:4">
       <c r="A43" s="1">
         <v>41</v>
       </c>
       <c r="B43" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="44" spans="1:2">
+        <v>44</v>
+      </c>
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4">
       <c r="A44" s="1">
         <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="45" spans="1:2">
+        <v>45</v>
+      </c>
+      <c r="C44" t="s">
+        <v>93</v>
+      </c>
+      <c r="D44" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="45" spans="1:4">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="46" spans="1:2">
+        <v>46</v>
+      </c>
+      <c r="C45" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:4">
       <c r="A46" s="1">
         <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="47" spans="1:2">
+        <v>47</v>
+      </c>
+      <c r="C46" t="s">
+        <v>95</v>
+      </c>
+      <c r="D46" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="47" spans="1:4">
       <c r="A47" s="1">
         <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="48" spans="1:2">
+        <v>48</v>
+      </c>
+      <c r="C47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D47" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="48" spans="1:4">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="49" spans="1:2">
+        <v>49</v>
+      </c>
+      <c r="C48" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="50" spans="1:2">
+        <v>50</v>
+      </c>
+      <c r="C49" t="s">
+        <v>98</v>
+      </c>
+      <c r="D49" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:2">
+        <v>51</v>
+      </c>
+      <c r="C50" t="s">
+        <v>99</v>
+      </c>
+      <c r="D50" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="51" spans="1:4">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" t="s">
-        <v>2</v>
+        <v>52</v>
+      </c>
+      <c r="C51" t="s">
+        <v>100</v>
+      </c>
+      <c r="D51" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>

</xml_diff>